<commit_message>
chore: update Tips & Features documentation and remove temporary file
</commit_message>
<xml_diff>
--- a/cypress/support/documentation/Tips & Features.xlsx
+++ b/cypress/support/documentation/Tips & Features.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://btgroupcloud-my.sharepoint.com/personal/sam_2_greenwood_bt_com/Documents/Desktop/Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\615594345\Downloads\Cypress\Cypress\cypress\support\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{40042E3D-8ABA-4C7D-B428-F123F6B02A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903851DD-1BC1-4DFE-809A-CAFAA4860496}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982E9480-89F5-4B5F-9798-62882964BF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{2A61AFED-7851-4191-AFD0-75E1D754F0B5}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="129">
   <si>
     <t>VS Code</t>
   </si>
@@ -382,12 +382,6 @@
   <si>
     <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>Specified which files to ignore when we push our changes up to GitHub
-We don’t need every file in our project to be pushed up to GitHub, the node_modules folder contains thousands of files and can be over 100mb
-Our package.json contains everything we need to build out project, using command npm install created everything we need including node_modules locally
-We generate our own node_modules locally, and GitHub generates its own node_modules when running the CI workflows</t>
   </si>
   <si>
     <t>Any file changes we make, prior to committing them, can be undone from the Source Control area by clicking the unstage changes icon</t>
@@ -422,6 +416,52 @@
   <si>
     <t>missing brackets etc
 Double clicking on any problem will direct  us to the code causing the issue</t>
+  </si>
+  <si>
+    <t>Format Code</t>
+  </si>
+  <si>
+    <t>Shift + Alt + F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formats code in the window that’s currently </t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>Go to definition</t>
+  </si>
+  <si>
+    <t>Placing your cursor on a method and pressing F12 will direct you to the underlying code for this method</t>
+  </si>
+  <si>
+    <t>Ctrl + /</t>
+  </si>
+  <si>
+    <t>Comment/Uncomment code</t>
+  </si>
+  <si>
+    <t>Highlight the code you want to comment/uncomment then press ctrl &amp; /</t>
+  </si>
+  <si>
+    <t>Open command palette</t>
+  </si>
+  <si>
+    <t>Ctrl + shift + p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open the command palette which gives access to any vs code command
+</t>
+  </si>
+  <si>
+    <t>Shortcut</t>
+  </si>
+  <si>
+    <t>Specifies which files to ignore when we push our changes up to GitHub
+We don’t need every file in our project to be pushed up to GitHub, the node_modules folder contains thousands of files and can be over 100mb
+Our package.json contains everything we need to build out project, using command npm install created everything we need including node_modules locally
+We generate our own node_modules locally, and GitHub generates its own node_modules when running the CI workflows</t>
   </si>
 </sst>
 </file>
@@ -502,20 +542,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,7 +894,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>106</v>
@@ -940,173 +980,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF020C26-3535-46E1-9C5C-2E1A03346BAE}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>120</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1125,7 +1214,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1255,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,10 +1267,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
     </row>
@@ -1282,7 +1371,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,10 +1384,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
     </row>
@@ -1309,7 +1398,7 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="3"/>
@@ -1428,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD16F4FE-2A57-4522-87AD-5FCA719C4928}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,10 +1531,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
     </row>
@@ -1456,26 +1545,26 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1575,7 +1664,7 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B15" s="2"/>

</xml_diff>